<commit_message>
Task: refactored the module PandaExtractData and added unit test cases for same module
</commit_message>
<xml_diff>
--- a/tests/input_excel_files/division_1000values.xlsx
+++ b/tests/input_excel_files/division_1000values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thulasigovardhan/Documents/NJIT Fall 2021/IS601/csv input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E086875-5FFC-1647-8C83-CB828E45E794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F077FC92-1548-B847-B8AD-ED9450E35CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E3D58822-AF80-AC4F-9AB7-178C3CB5323F}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,25 +415,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <f>A2/B2</f>
+        <f>A3/B3</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
-        <f>A2/B2</f>
+        <f>A3/B3</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>